<commit_message>
* Update localize string.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/StringTable.xlsx
+++ b/example/BuildSchema/Tables/StringTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\src\Devarc.Builder\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A07B6-676F-45DF-863E-6704A1B4AA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5735F8-E0C6-4F47-A303-24F605726B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="2235" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="LString" sheetId="2" r:id="rId1"/>
@@ -36,43 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>key</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_SHOOT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_ATTACK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ko</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>en</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>String ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Korean</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -95,6 +59,26 @@
   </si>
   <si>
     <t>Shooting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillname_attack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillname_shoot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chinese</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Japanese</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -494,80 +478,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.875" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
+    <col min="2" max="5" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Update string table.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/StringTable.xlsx
+++ b/example/BuildSchema/Tables/StringTable.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5735F8-E0C6-4F47-A303-24F605726B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D62300-E490-4957-9A63-0D843A5BD173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="LString" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LString!$A$1:$E$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,63 +39,134 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Korean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>English</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal Attack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>평타</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사격</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shooting</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillname_attack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillname_shoot</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Chinese</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Japanese</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_attack</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>攻</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>撃</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>攻</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>击</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>반격</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>反</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>击</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>反</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>撃</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter Attack</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_counter</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -110,8 +184,22 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,8 +211,14 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -147,21 +241,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -478,71 +715,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="18.25" customWidth="1"/>
+    <col min="1" max="1" width="17.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="18.25" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="C3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <autoFilter ref="A1:E3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Update framework tools.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/StringTable.xlsx
+++ b/example/BuildSchema/Tables/StringTable.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maoshy/Documents/Projects/branches/devarc/example/BuildSchema/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FED3D7-F9E6-4B63-8D8E-274513286651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F961959F-5D8E-CA4A-9E48-DA8E5EAC8232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="LString" sheetId="2" r:id="rId1"/>
-    <sheet name="LString@built-in" sheetId="3" r:id="rId2"/>
+    <sheet name="LString@resource" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LString!$A$1:$E$3</definedName>
@@ -170,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,9 +455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -495,7 +495,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -601,7 +601,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -743,7 +743,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,15 +753,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="5" width="31.875" style="2" customWidth="1"/>
+    <col min="1" max="5" width="31.83203125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -779,7 +779,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -796,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
@@ -824,15 +824,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B7A05-21C3-44AC-BC6A-CCFD4B632868}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="5" width="31.875" style="2" customWidth="1"/>
+    <col min="1" max="5" width="31.83203125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -850,7 +850,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>

</xml_diff>